<commit_message>
Memperbarui coding utama dan membuat struk
</commit_message>
<xml_diff>
--- a/Tubes.xlsx
+++ b/Tubes.xlsx
@@ -437,7 +437,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:NO11"/>
+  <dimension ref="A1:NO14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F10" sqref="F10"/>
@@ -672,6 +672,66 @@
         </is>
       </c>
     </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>12</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>btara</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>123</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>13/06/2022 10:40:05</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>13</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>btara</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>123</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>14/06/2022 12:05:49</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>14</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>aaa</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>aaa</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>14/06/2022 19:16:43</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>